<commit_message>
add: put and delete
</commit_message>
<xml_diff>
--- a/test-case/plantillaBack.xlsx
+++ b/test-case/plantillaBack.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Training\git\APIFW\test-case\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="35">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -121,7 +121,16 @@
     <t>/users</t>
   </si>
   <si>
-    <t>{name:victor, job:leader}</t>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>{name:Edwin, job:zion resident}</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>{}</t>
   </si>
 </sst>
 </file>
@@ -732,7 +741,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +877,7 @@
         <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H5" s="3">
         <v>200</v>
@@ -882,18 +891,62 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="B6" s="3">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="3">
+        <v>200</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G7" s="3"/>
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="3">
+        <v>204</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>